<commit_message>
top 100 Unis and Uni Job Listing CV Uni matching was installed
</commit_message>
<xml_diff>
--- a/upload_files/CV1__booking_data_engineer_senior.xlsx
+++ b/upload_files/CV1__booking_data_engineer_senior.xlsx
@@ -868,7 +868,7 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -876,7 +876,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:11">

</xml_diff>